<commit_message>
NIEM EM 3.1 IEPD Data Model Attributes 1.3 Phase I
Existing NIEM EM 3.0 has been mapped to DHS conceptual data modal
</commit_message>
<xml_diff>
--- a/NIEM EM 3.1 IEPD Data Model Attributes _v1.3 Phase I.xlsx
+++ b/NIEM EM 3.1 IEPD Data Model Attributes _v1.3 Phase I.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'NIEM EM3.0 Typing'!$A$1:$A$366</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcOnSave="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -2753,6 +2753,7 @@
       <u/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2760,6 +2761,7 @@
       <u/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3418,6 +3420,14 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -3437,6 +3447,192 @@
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3492,28 +3688,13 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3524,43 +3705,9 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+        <bottom style="thin">
           <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3597,151 +3744,6 @@
           <color indexed="64"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3880,12 +3882,12 @@
     <sortCondition ref="B1:B365"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" name="Attribute Name" totalsRowFunction="count" dataDxfId="11" totalsRowDxfId="5"/>
-    <tableColumn id="6" name="Parent Type" dataDxfId="10" totalsRowDxfId="4"/>
-    <tableColumn id="2" name="Attribute Type" dataDxfId="9" totalsRowDxfId="3"/>
-    <tableColumn id="3" name="Description" dataDxfId="8" totalsRowDxfId="2"/>
-    <tableColumn id="5" name="Standard Name" dataDxfId="7" totalsRowDxfId="1"/>
-    <tableColumn id="4" name="Comment/Feedback" dataDxfId="6" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Attribute Name" totalsRowFunction="count" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="6" name="Parent Type" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" name="Attribute Type" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" name="Description" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="5" name="Standard Name" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="4" name="Comment/Feedback" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>

</xml_diff>